<commit_message>
add fund for upload excel file ed/ned
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/edned_template.xlsx
+++ b/src/main/webapp/resources/files/edned_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>TMTID</t>
   </si>
@@ -35,6 +35,15 @@
   </si>
   <si>
     <t>TMTID จะต้องอ้างอิงรหัสที่มีในฐานกลาง,DATEIN ควร format excel เป็น date,ISED ค่าที่เป็นไปได้คือ E,N,E*</t>
+  </si>
+  <si>
+    <t>FUNDCODE</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>FUNDCODE จะต้องมีในฐานข้อมูล</t>
   </si>
 </sst>
 </file>
@@ -377,15 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,8 +404,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>497099</v>
       </c>
@@ -407,10 +419,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>180175</v>
       </c>
@@ -420,8 +435,14 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>203965</v>
       </c>
@@ -430,6 +451,9 @@
       </c>
       <c r="C4" t="s">
         <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change fund to right
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/edned_template.xlsx
+++ b/src/main/webapp/resources/files/edned_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,13 +37,13 @@
     <t>TMTID จะต้องอ้างอิงรหัสที่มีในฐานกลาง,DATEIN ควร format excel เป็น date,ISED ค่าที่เป็นไปได้คือ E,N,E*</t>
   </si>
   <si>
-    <t>FUNDCODE</t>
-  </si>
-  <si>
     <t>UC</t>
   </si>
   <si>
-    <t>FUNDCODE จะต้องมีในฐานข้อมูล</t>
+    <t>RIGHTID</t>
+  </si>
+  <si>
+    <t>RIGHTID จะต้องมีในฐานข้อมูล</t>
   </si>
 </sst>
 </file>
@@ -392,9 +392,9 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,10 +405,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>497099</v>
       </c>
@@ -419,13 +419,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>180175</v>
       </c>
@@ -436,13 +436,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>203965</v>
       </c>
@@ -453,7 +453,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>